<commit_message>
ADD Fomulario de contacto y arreglos varios
Co-authored-by: AlejandroRS123 <AlejandroRS123@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/uploads/productes.xlsx
+++ b/uploads/productes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">img/raton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A004</t>
   </si>
 </sst>
 </file>
@@ -92,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,6 +119,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -169,11 +179,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,11 +191,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,7 +325,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -412,12 +422,35 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>20</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="5"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>